<commit_message>
Updating Sample Spreadsheet with Anchored Images
</commit_message>
<xml_diff>
--- a/MESS/MESS.Data/TestData/WorkInstructions/MESS-Excel-Template.xlsx
+++ b/MESS/MESS.Data/TestData/WorkInstructions/MESS-Excel-Template.xlsx
@@ -1,55 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb150f21903e2344/Documents/Valparaiso University/CS358/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sthyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{4E430D6B-947B-4295-B877-85AD49997D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CB3D6A8-A222-4B7E-8878-AD3C6FADE0F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8584F8-29D0-4FB2-8DAF-B5C869AF8299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="2">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-    <bk>
-      <rc t="1" v="1"/>
-    </bk>
-  </valueMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,73 +458,97 @@
 </styleSheet>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-</richValueRels>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>442305</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D80D4D3-F0E7-88DF-94CF-15D49D30CADD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6130290" y="2708910"/>
+          <a:ext cx="662940" cy="442305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1535431</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1023222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D287A6C6-0CA0-9AB6-2CFD-28FDBCAA5C04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7917181" y="3646172"/>
+          <a:ext cx="1535430" cy="1023220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -763,19 +754,19 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="45.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.3984375" customWidth="1"/>
-    <col min="4" max="4" width="26.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.38671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.38671875" customWidth="1"/>
+    <col min="4" max="4" width="26.0546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +780,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -803,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -811,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -828,7 +819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="40.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="40.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -839,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="39.4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -850,7 +841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -861,7 +852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="39.4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -871,11 +862,8 @@
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="38.65" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:5" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -886,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="90.4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="86.1" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -896,44 +884,41 @@
       <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -944,5 +929,12 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{a06a2aab-1ff3-4080-b3c6-82af45ab1506}" enabled="1" method="Standard" siteId="{078256a4-c4a0-4e95-b107-2ae7d5db8581}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>